<commit_message>
Login - arreglo errores
Se arreglan errores derivados de insertar un valor alfabetico en el campo del DNI. devolvía InvalidError
</commit_message>
<xml_diff>
--- a/Dat/BaseDeDatosUsuarios.xlsx
+++ b/Dat/BaseDeDatosUsuarios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -64,6 +64,9 @@
     <t>9</t>
   </si>
   <si>
+    <t>Juanito</t>
+  </si>
+  <si>
     <t>carro</t>
   </si>
   <si>
@@ -74,6 +77,12 @@
   </si>
   <si>
     <t>Maria</t>
+  </si>
+  <si>
+    <t>Los palotes</t>
+  </si>
+  <si>
+    <t>hola</t>
   </si>
   <si>
     <t>H</t>
@@ -443,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,13 +501,13 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>1234</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -516,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -527,13 +536,13 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>1234</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F3">
         <v>21</v>
@@ -551,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -562,13 +571,13 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>1234</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F4">
         <v>33</v>
@@ -586,7 +595,7 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -597,13 +606,13 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>21</v>
@@ -621,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -634,11 +643,11 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
+      <c r="D6">
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>9</v>
@@ -656,7 +665,42 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>123456789</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>23</v>
+      </c>
+      <c r="F7">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <v>168</v>
+      </c>
+      <c r="H7">
+        <v>55</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>